<commit_message>
updated realtime zip and scripts
</commit_message>
<xml_diff>
--- a/retail/Azureresources.xlsx
+++ b/retail/Azureresources.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\priyanka\IOT\MSFT-Repo\Azure-Analytics-and-AI-Engagement\retail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D30B59AC-DF4F-4709-9058-4A53CE7F70FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCFBB87-494D-41A4-A13F-973511788C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Azureresources" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="131">
   <si>
     <t>NAME</t>
   </si>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1252,11 +1252,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,6 +1716,9 @@
       <c r="B41" t="s">
         <v>63</v>
       </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1773,6 +1776,9 @@
       </c>
       <c r="B46" t="s">
         <v>71</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>